<commit_message>
Don't know why there are so many changes
</commit_message>
<xml_diff>
--- a/pythia_ig/output/CodeSystem-EvalReason.xlsx
+++ b/pythia_ig/output/CodeSystem-EvalReason.xlsx
@@ -36,7 +36,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>EvalReason</t>
+    <t>EvalReasonCS</t>
   </si>
   <si>
     <t>Title</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-30T19:45:10-04:00</t>
+    <t>2024-04-30T22:06:35-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>